<commit_message>
Added news section to home screen and various resource lists to resources screen. Added interactive map template and developed functions for scoring a user's water test results. Structured the layout of user data, geographic data, contaminant and other data in the resources folder. Cleaned UI and unified colors/theme.
</commit_message>
<xml_diff>
--- a/resources/InAppResources.xlsx
+++ b/resources/InAppResources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\Code\Local Projects\GSSTeam12Project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09CB3080-C676-4ABB-B374-1D30BCA59507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B05ACB-A408-46C5-A847-8B7AE54C0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{79CB1594-F4F6-8D42-85D2-FFEA54BCE5B6}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Display Name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>NJ DOH Water Quality Overview</t>
   </si>
@@ -56,28 +50,211 @@
     <t xml:space="preserve">https://www.njwatercheck.com/SystemFinder </t>
   </si>
   <si>
-    <t>NJDEP Data Miner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://njems.nj.gov/DataMiner/Search/SearchByCategory?isExternal=y&amp;getCategory=y&amp;catName=Water+Supply+and+Geoscience </t>
-  </si>
-  <si>
     <t>NJ American Water Lead Service Line Map</t>
   </si>
   <si>
     <t>https://amwater.com/njaw/Water-Quality/Lead-and-Drinking-Water/</t>
   </si>
   <si>
-    <t>NJ American Water Consumer Confidence Reports</t>
-  </si>
-  <si>
-    <t>https://amwater.com/corp/Water-Quality-Wastewater-Service/water-quality-reports</t>
-  </si>
-  <si>
     <t>NJ Water Works Latest News Page</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.jerseywaterworks.org/latest-news/ </t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>General Educational</t>
+  </si>
+  <si>
+    <t>External Tool</t>
+  </si>
+  <si>
+    <t>News and Events</t>
+  </si>
+  <si>
+    <t>NJDEP News Releases</t>
+  </si>
+  <si>
+    <t>https://dep.nj.gov/newsrel/</t>
+  </si>
+  <si>
+    <t>NJ DOH Public Resources</t>
+  </si>
+  <si>
+    <t>https://www.nj.gov/health/ceohs/environmental-occupational/drinking-water-public-health/</t>
+  </si>
+  <si>
+    <t>https://dep.nj.gov/lead/water/</t>
+  </si>
+  <si>
+    <t>Lead and Drinking Water</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/mercury/basic-information-about-mercury</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/lead/learn-about-lead</t>
+  </si>
+  <si>
+    <t>Contaminants</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/nutrientpollution</t>
+  </si>
+  <si>
+    <t>Nutrient Pollution</t>
+  </si>
+  <si>
+    <t>EWG Guide to Safe Drinking Water</t>
+  </si>
+  <si>
+    <t>https://static.ewg.org/ewg-tip-sheets/EWG-SafeDrinkingWaterGuide.pdf</t>
+  </si>
+  <si>
+    <t>https://nj211.org/water-bill-assistance-programs</t>
+  </si>
+  <si>
+    <t>State Programs</t>
+  </si>
+  <si>
+    <t>Water Bill Assistance Programs</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/sites/default/files/2015-11/documents/2005_09_14_faq_fs_homewatertesting.pdf</t>
+  </si>
+  <si>
+    <t>EPA Home Water Testing Facts</t>
+  </si>
+  <si>
+    <t>EPA How's My Waterway</t>
+  </si>
+  <si>
+    <t>https://mywaterway.epa.gov/state/NJ/water-quality-overview</t>
+  </si>
+  <si>
+    <t>https://www.ewg.org/tapwater/</t>
+  </si>
+  <si>
+    <t>Environmental Working Group (EWG) National Tap Water Database</t>
+  </si>
+  <si>
+    <t>Feedback and Complaints</t>
+  </si>
+  <si>
+    <t>https://www.nj.gov/dep/watersupply/pwq-complaint.html</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/sites/default/files/2015-04/documents/epa816f04030.pdf</t>
+  </si>
+  <si>
+    <t>Understanding the Safe Drinking Water Act (SDWA)</t>
+  </si>
+  <si>
+    <t>NJDEP Public Water Quality Complaints</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>njdep_icon.png</t>
+  </si>
+  <si>
+    <t>epa_icon.png</t>
+  </si>
+  <si>
+    <t>tap_water_contamination_icon.jpg</t>
+  </si>
+  <si>
+    <t>lead_icon.png</t>
+  </si>
+  <si>
+    <t>nutrient_contamination_icon.jpg</t>
+  </si>
+  <si>
+    <t>lead_2_icon.jpg</t>
+  </si>
+  <si>
+    <t>jww_icon.png</t>
+  </si>
+  <si>
+    <t>nj_am_water_icon.jpg</t>
+  </si>
+  <si>
+    <t>njdoh_icon.jpg</t>
+  </si>
+  <si>
+    <t>mercury_icon.jpg</t>
+  </si>
+  <si>
+    <t>ewg_tap_water_database_icon.png.jpg</t>
+  </si>
+  <si>
+    <t>Display Name (en)</t>
+  </si>
+  <si>
+    <t>Display Name (es)</t>
+  </si>
+  <si>
+    <t>NJ American Water Mapa de línea de servicio principal</t>
+  </si>
+  <si>
+    <t>NJ Water Check Herramienta de búsqueda del sistema</t>
+  </si>
+  <si>
+    <t>Descripción general de la calidad del agua del NJ DOH</t>
+  </si>
+  <si>
+    <t>NJ Water Works Página de últimas noticias</t>
+  </si>
+  <si>
+    <t>NJDEP Comunicados de prensa</t>
+  </si>
+  <si>
+    <t>NJ DOH Recursos públicos</t>
+  </si>
+  <si>
+    <t>Plomo y agua potable</t>
+  </si>
+  <si>
+    <t>Mercurio</t>
+  </si>
+  <si>
+    <t>Plomo</t>
+  </si>
+  <si>
+    <t>Contaminación por nutrientes</t>
+  </si>
+  <si>
+    <t>EWG Guía para el agua potable segura</t>
+  </si>
+  <si>
+    <t>Programas de asistencia para facturas de agua</t>
+  </si>
+  <si>
+    <t>EPA Datos sobre las pruebas de agua en el hogar</t>
+  </si>
+  <si>
+    <t>EPA ¿Cómo está mi canal?</t>
+  </si>
+  <si>
+    <t>Environmental Working Group (EWG) Base de datos nacional de agua del grifo</t>
+  </si>
+  <si>
+    <t>NJDEP Quejas públicas sobre la calidad del agua</t>
+  </si>
+  <si>
+    <t>Comprender la Ley de Agua Potable Segura</t>
   </si>
 </sst>
 </file>
@@ -460,82 +637,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15283A4C-DCCB-CA4D-8386-5A7DAB63CBE2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="1" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="22.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2B826879-2083-7F44-8D73-206DE5578C83}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{BB6AAD11-948B-A743-B459-9F729FFD7ED2}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{F6A84A29-243B-B44D-9AF1-68BDF9E1EBDE}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{7EC13A39-44C0-F64F-B077-0656232CA0B3}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{8723BEF4-BEE9-A247-92D2-FA00FEE02670}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{DA4A83B6-9B7C-B442-9494-5DFAFB1DA055}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2B826879-2083-7F44-8D73-206DE5578C83}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{BB6AAD11-948B-A743-B459-9F729FFD7ED2}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{7EC13A39-44C0-F64F-B077-0656232CA0B3}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{DA4A83B6-9B7C-B442-9494-5DFAFB1DA055}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{35BF9781-C55C-43C4-8CBB-49A48CEF644F}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{5D65BBE5-F807-4419-996F-3F15010137D1}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{88F2414A-D2C9-4E63-B74B-D7FADA1DAA43}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{6E60E3E7-9747-4C9D-9874-FE43384273FA}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{41A9326F-E630-47FF-ADAB-5DE30E18E8D8}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{6A70A3CA-0EC0-4055-A797-9EF8D9DA312C}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{31A760C1-F826-45AD-93A9-A638FC831131}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{8D17D0B6-16E1-46A2-A2A1-678DCF91F625}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{71D00D66-16CE-4AE0-B4E8-11BC7D80E08A}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{3F4BE674-D4C5-421B-B1F5-DC5174DEAA40}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{C73171B7-E290-40CA-A754-4F1E370496E2}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{1833AF79-080C-413C-BD6F-8ED6EE1EDAC6}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{B3B1CD7C-459E-49FD-BC87-23F28B63A8FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>